<commit_message>
cg: bsa - update district list.
</commit_message>
<xml_diff>
--- a/ONCHO/Breeding Site Survey/Congo/2021/cg_oncho_bsc_2_capture_202107.xlsx
+++ b/ONCHO/Breeding Site Survey/Congo/2021/cg_oncho_bsc_2_capture_202107.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Repositories\WHO\dsa-forms\ONCHO\Breeding Site Survey\Congo\2021\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F9C97B-DA61-4A7F-8781-00A6DD3EAC65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9DAC973-C0FC-45AA-8BA0-98ED25854F96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="429" uniqueCount="184">
   <si>
     <t>form_title</t>
   </si>
@@ -251,12 +251,6 @@
     <t>Dolisie</t>
   </si>
   <si>
-    <t>Goma Tse-Tse</t>
-  </si>
-  <si>
-    <t>Igne-Ngabe-Mayama</t>
-  </si>
-  <si>
     <t>Kibangou</t>
   </si>
   <si>
@@ -273,9 +267,6 @@
   </si>
   <si>
     <t>Loudima</t>
-  </si>
-  <si>
-    <t>Loutete</t>
   </si>
   <si>
     <t>Madingou</t>
@@ -522,6 +513,87 @@
   </si>
   <si>
     <t>cg_oncho_bsc_2_capture_202107</t>
+  </si>
+  <si>
+    <t>Brazzaville</t>
+  </si>
+  <si>
+    <t>Cuvette</t>
+  </si>
+  <si>
+    <t>Kouilou</t>
+  </si>
+  <si>
+    <t>Plateaux</t>
+  </si>
+  <si>
+    <t>Loutété</t>
+  </si>
+  <si>
+    <t>Bacongo</t>
+  </si>
+  <si>
+    <t>Djiri</t>
+  </si>
+  <si>
+    <t>Ile Mbamou</t>
+  </si>
+  <si>
+    <t>Madibou</t>
+  </si>
+  <si>
+    <t>Makélékélé</t>
+  </si>
+  <si>
+    <t>Mfilou</t>
+  </si>
+  <si>
+    <t>Moungali</t>
+  </si>
+  <si>
+    <t>Ouenzé</t>
+  </si>
+  <si>
+    <t>Poto-Poto</t>
+  </si>
+  <si>
+    <t>Talangai</t>
+  </si>
+  <si>
+    <t>Mossaka</t>
+  </si>
+  <si>
+    <t>Owando</t>
+  </si>
+  <si>
+    <t>Oyo-Alima</t>
+  </si>
+  <si>
+    <t>Hinda</t>
+  </si>
+  <si>
+    <t>Madingo-Kayes-Nzambi</t>
+  </si>
+  <si>
+    <t>Mvouti-Kakamoeka</t>
+  </si>
+  <si>
+    <t>Abala</t>
+  </si>
+  <si>
+    <t>Djambala</t>
+  </si>
+  <si>
+    <t>Gamboma</t>
+  </si>
+  <si>
+    <t>Ngo-Mpouya</t>
+  </si>
+  <si>
+    <t>Goma Tsé-Tsé</t>
+  </si>
+  <si>
+    <t>Igné-Ngabe-Mayama</t>
   </si>
 </sst>
 </file>
@@ -1012,7 +1084,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -1073,10 +1145,10 @@
         <v>12</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" ht="31.35" x14ac:dyDescent="0.55000000000000004">
@@ -1112,7 +1184,7 @@
         <v>62</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C3" s="9" t="s">
         <v>63</v>
@@ -1150,7 +1222,7 @@
       </c>
       <c r="K4" s="10"/>
       <c r="L4" s="10" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="5" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -1161,7 +1233,7 @@
         <v>55</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="12"/>
@@ -1180,10 +1252,10 @@
         <v>21</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="10"/>
@@ -1202,10 +1274,10 @@
         <v>21</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="10"/>
@@ -1219,13 +1291,13 @@
     </row>
     <row r="8" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="8" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D8" s="9"/>
       <c r="E8" s="10"/>
@@ -1261,16 +1333,16 @@
     </row>
     <row r="10" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="8" t="s">
+        <v>143</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>146</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C10" s="9" t="s">
-        <v>148</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>149</v>
       </c>
       <c r="E10" s="12"/>
       <c r="F10" s="19"/>
@@ -1299,7 +1371,7 @@
       <c r="D11" s="9"/>
       <c r="E11" s="10"/>
       <c r="F11" s="8" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="G11" s="13" t="s">
         <v>50</v>
@@ -1317,20 +1389,20 @@
         <v>15</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E12" s="10"/>
       <c r="F12" s="8" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="G12" s="13" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
@@ -1356,17 +1428,17 @@
     </row>
     <row r="14" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A14" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B14" s="15" t="s">
+        <v>97</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>100</v>
-      </c>
-      <c r="C14" s="9" t="s">
-        <v>103</v>
       </c>
       <c r="D14" s="9"/>
       <c r="E14" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F14" s="8"/>
       <c r="G14" s="13"/>
@@ -1381,14 +1453,14 @@
         <v>41</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D15" s="9"/>
       <c r="E15" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="13"/>
@@ -1405,7 +1477,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C16" s="9" t="s">
         <v>61</v>
@@ -1427,7 +1499,7 @@
         <v>49</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>54</v>
@@ -1446,7 +1518,7 @@
     </row>
     <row r="18" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A18" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B18" s="15"/>
       <c r="C18" s="9"/>
@@ -1476,22 +1548,22 @@
     </row>
     <row r="20" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A20" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="D20" s="9"/>
       <c r="E20" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F20" s="8"/>
       <c r="G20" s="13"/>
       <c r="H20" s="10" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="I20" s="10"/>
       <c r="J20" s="6"/>
@@ -1503,14 +1575,14 @@
         <v>41</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="C21" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D21" s="9"/>
       <c r="E21" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F21" s="8"/>
       <c r="G21" s="13"/>
@@ -1527,7 +1599,7 @@
         <v>15</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="C22" s="9" t="s">
         <v>61</v>
@@ -1549,7 +1621,7 @@
         <v>49</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="C23" s="9" t="s">
         <v>54</v>
@@ -1568,7 +1640,7 @@
     </row>
     <row r="24" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A24" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="9"/>
@@ -1598,22 +1670,22 @@
     </row>
     <row r="26" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A26" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D26" s="9"/>
       <c r="E26" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F26" s="8"/>
       <c r="G26" s="13"/>
       <c r="H26" s="10" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="I26" s="10"/>
       <c r="J26" s="6"/>
@@ -1625,14 +1697,14 @@
         <v>41</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="C27" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D27" s="9"/>
       <c r="E27" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F27" s="8"/>
       <c r="G27" s="13"/>
@@ -1649,7 +1721,7 @@
         <v>15</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C28" s="9" t="s">
         <v>61</v>
@@ -1671,7 +1743,7 @@
         <v>49</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C29" s="9" t="s">
         <v>54</v>
@@ -1690,7 +1762,7 @@
     </row>
     <row r="30" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A30" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B30" s="15"/>
       <c r="C30" s="9"/>
@@ -1720,22 +1792,22 @@
     </row>
     <row r="32" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A32" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="D32" s="9"/>
       <c r="E32" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="13"/>
       <c r="H32" s="10" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="I32" s="10"/>
       <c r="J32" s="6"/>
@@ -1747,14 +1819,14 @@
         <v>41</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C33" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D33" s="9"/>
       <c r="E33" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F33" s="8"/>
       <c r="G33" s="13"/>
@@ -1771,7 +1843,7 @@
         <v>15</v>
       </c>
       <c r="B34" s="15" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C34" s="9" t="s">
         <v>61</v>
@@ -1793,7 +1865,7 @@
         <v>49</v>
       </c>
       <c r="B35" s="15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>54</v>
@@ -1812,7 +1884,7 @@
     </row>
     <row r="36" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A36" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B36" s="15"/>
       <c r="C36" s="9"/>
@@ -1842,22 +1914,22 @@
     </row>
     <row r="38" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A38" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B38" s="15" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C38" s="9" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="D38" s="9"/>
       <c r="E38" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F38" s="8"/>
       <c r="G38" s="13"/>
       <c r="H38" s="10" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="I38" s="10"/>
       <c r="J38" s="6"/>
@@ -1869,14 +1941,14 @@
         <v>41</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D39" s="9"/>
       <c r="E39" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F39" s="8"/>
       <c r="G39" s="13"/>
@@ -1893,7 +1965,7 @@
         <v>15</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>61</v>
@@ -1915,7 +1987,7 @@
         <v>49</v>
       </c>
       <c r="B41" s="15" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C41" s="9" t="s">
         <v>54</v>
@@ -1934,7 +2006,7 @@
     </row>
     <row r="42" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A42" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B42" s="15"/>
       <c r="C42" s="9"/>
@@ -1964,22 +2036,22 @@
     </row>
     <row r="44" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A44" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B44" s="15" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C44" s="9" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="D44" s="9"/>
       <c r="E44" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F44" s="8"/>
       <c r="G44" s="13"/>
       <c r="H44" s="10" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="I44" s="10"/>
       <c r="J44" s="6"/>
@@ -1991,14 +2063,14 @@
         <v>41</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D45" s="9"/>
       <c r="E45" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F45" s="8"/>
       <c r="G45" s="13"/>
@@ -2015,7 +2087,7 @@
         <v>15</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C46" s="9" t="s">
         <v>61</v>
@@ -2037,7 +2109,7 @@
         <v>49</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>54</v>
@@ -2056,7 +2128,7 @@
     </row>
     <row r="48" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A48" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B48" s="15"/>
       <c r="C48" s="9"/>
@@ -2086,22 +2158,22 @@
     </row>
     <row r="50" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A50" s="20" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="B50" s="15" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C50" s="9" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="D50" s="9"/>
       <c r="E50" s="10" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="F50" s="8"/>
       <c r="G50" s="13"/>
       <c r="H50" s="10" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="I50" s="10"/>
       <c r="J50" s="6"/>
@@ -2113,14 +2185,14 @@
         <v>41</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C51" s="9" t="s">
         <v>28</v>
       </c>
       <c r="D51" s="9"/>
       <c r="E51" s="10" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="F51" s="8"/>
       <c r="G51" s="13"/>
@@ -2137,7 +2209,7 @@
         <v>15</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C52" s="9" t="s">
         <v>61</v>
@@ -2159,7 +2231,7 @@
         <v>49</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C53" s="9" t="s">
         <v>54</v>
@@ -2178,7 +2250,7 @@
     </row>
     <row r="54" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.4">
       <c r="A54" s="20" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B54" s="15"/>
       <c r="C54" s="9"/>
@@ -2211,10 +2283,10 @@
         <v>21</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C56" s="16" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="D56" s="16"/>
       <c r="E56" s="12"/>
@@ -2222,7 +2294,7 @@
       <c r="G56" s="17"/>
       <c r="H56" s="12"/>
       <c r="I56" s="12" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="J56" s="6"/>
       <c r="K56" s="12"/>
@@ -2324,11 +2396,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A38" sqref="A38:A58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.7" x14ac:dyDescent="0.55000000000000004"/>
@@ -2511,10 +2583,10 @@
         <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>68</v>
+        <v>157</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>157</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2522,65 +2594,53 @@
         <v>66</v>
       </c>
       <c r="B17" t="s">
-        <v>69</v>
+        <v>158</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
-        <v>71</v>
+        <v>159</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
-      </c>
-      <c r="D18" t="s">
-        <v>69</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B19" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="C19" t="s">
-        <v>72</v>
-      </c>
-      <c r="D19" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B20" t="s">
-        <v>73</v>
+        <v>160</v>
       </c>
       <c r="C20" t="s">
-        <v>73</v>
-      </c>
-      <c r="D20" t="s">
-        <v>69</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>74</v>
-      </c>
-      <c r="D21" t="s">
         <v>69</v>
       </c>
     </row>
@@ -2589,13 +2649,13 @@
         <v>70</v>
       </c>
       <c r="B22" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="C22" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2603,13 +2663,13 @@
         <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>76</v>
+        <v>161</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>161</v>
       </c>
       <c r="D23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2617,13 +2677,13 @@
         <v>70</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C24" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2631,13 +2691,13 @@
         <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="D25" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2645,13 +2705,13 @@
         <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="C26" t="s">
-        <v>79</v>
+        <v>84</v>
       </c>
       <c r="D26" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2659,13 +2719,13 @@
         <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>80</v>
+        <v>162</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>162</v>
       </c>
       <c r="D27" t="s">
-        <v>67</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2673,13 +2733,13 @@
         <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>163</v>
       </c>
       <c r="C28" t="s">
-        <v>81</v>
+        <v>163</v>
       </c>
       <c r="D28" t="s">
-        <v>67</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2687,13 +2747,13 @@
         <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>82</v>
+        <v>164</v>
       </c>
       <c r="C29" t="s">
-        <v>82</v>
+        <v>164</v>
       </c>
       <c r="D29" t="s">
-        <v>67</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2701,13 +2761,13 @@
         <v>70</v>
       </c>
       <c r="B30" t="s">
-        <v>83</v>
+        <v>165</v>
       </c>
       <c r="C30" t="s">
-        <v>83</v>
+        <v>165</v>
       </c>
       <c r="D30" t="s">
-        <v>68</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2715,13 +2775,13 @@
         <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>84</v>
+        <v>166</v>
       </c>
       <c r="C31" t="s">
-        <v>84</v>
+        <v>166</v>
       </c>
       <c r="D31" t="s">
-        <v>69</v>
+        <v>157</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2729,13 +2789,13 @@
         <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>85</v>
+        <v>167</v>
       </c>
       <c r="C32" t="s">
-        <v>85</v>
+        <v>167</v>
       </c>
       <c r="D32" t="s">
-        <v>68</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2743,13 +2803,13 @@
         <v>70</v>
       </c>
       <c r="B33" t="s">
-        <v>86</v>
+        <v>168</v>
       </c>
       <c r="C33" t="s">
-        <v>86</v>
+        <v>168</v>
       </c>
       <c r="D33" t="s">
-        <v>67</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -2757,18 +2817,354 @@
         <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>87</v>
+        <v>169</v>
       </c>
       <c r="C34" t="s">
-        <v>87</v>
+        <v>169</v>
       </c>
       <c r="D34" t="s">
-        <v>67</v>
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" t="s">
+        <v>170</v>
+      </c>
+      <c r="C35" t="s">
+        <v>170</v>
+      </c>
+      <c r="D35" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A36" t="s">
+        <v>70</v>
+      </c>
+      <c r="B36" t="s">
+        <v>171</v>
+      </c>
+      <c r="C36" t="s">
+        <v>171</v>
+      </c>
+      <c r="D36" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A37" t="s">
+        <v>70</v>
+      </c>
+      <c r="B37" t="s">
+        <v>172</v>
+      </c>
+      <c r="C37" t="s">
+        <v>172</v>
+      </c>
+      <c r="D37" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A38" t="s">
+        <v>70</v>
+      </c>
+      <c r="B38" t="s">
+        <v>173</v>
+      </c>
+      <c r="C38" t="s">
+        <v>173</v>
+      </c>
+      <c r="D38" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A39" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" t="s">
+        <v>174</v>
+      </c>
+      <c r="C39" t="s">
+        <v>174</v>
+      </c>
+      <c r="D39" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" t="s">
+        <v>175</v>
+      </c>
+      <c r="C40" t="s">
+        <v>175</v>
+      </c>
+      <c r="D40" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A41" t="s">
+        <v>70</v>
+      </c>
+      <c r="B41" t="s">
+        <v>176</v>
+      </c>
+      <c r="C41" t="s">
+        <v>176</v>
+      </c>
+      <c r="D41" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" t="s">
+        <v>70</v>
+      </c>
+      <c r="B42" t="s">
+        <v>177</v>
+      </c>
+      <c r="C42" t="s">
+        <v>177</v>
+      </c>
+      <c r="D42" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" t="s">
+        <v>70</v>
+      </c>
+      <c r="B43" t="s">
+        <v>72</v>
+      </c>
+      <c r="C43" t="s">
+        <v>72</v>
+      </c>
+      <c r="D43" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" t="s">
+        <v>73</v>
+      </c>
+      <c r="C44" t="s">
+        <v>73</v>
+      </c>
+      <c r="D44" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" t="s">
+        <v>74</v>
+      </c>
+      <c r="D45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A46" t="s">
+        <v>70</v>
+      </c>
+      <c r="B46" t="s">
+        <v>80</v>
+      </c>
+      <c r="C46" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A47" t="s">
+        <v>70</v>
+      </c>
+      <c r="B47" t="s">
+        <v>82</v>
+      </c>
+      <c r="C47" t="s">
+        <v>82</v>
+      </c>
+      <c r="D47" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A48" t="s">
+        <v>70</v>
+      </c>
+      <c r="B48" t="s">
+        <v>178</v>
+      </c>
+      <c r="C48" t="s">
+        <v>178</v>
+      </c>
+      <c r="D48" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A49" t="s">
+        <v>70</v>
+      </c>
+      <c r="B49" t="s">
+        <v>179</v>
+      </c>
+      <c r="C49" t="s">
+        <v>179</v>
+      </c>
+      <c r="D49" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" t="s">
+        <v>70</v>
+      </c>
+      <c r="B50" t="s">
+        <v>180</v>
+      </c>
+      <c r="C50" t="s">
+        <v>180</v>
+      </c>
+      <c r="D50" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" t="s">
+        <v>70</v>
+      </c>
+      <c r="B51" t="s">
+        <v>181</v>
+      </c>
+      <c r="C51" t="s">
+        <v>181</v>
+      </c>
+      <c r="D51" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A52" t="s">
+        <v>70</v>
+      </c>
+      <c r="B52" t="s">
+        <v>71</v>
+      </c>
+      <c r="C52" t="s">
+        <v>71</v>
+      </c>
+      <c r="D52" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A53" t="s">
+        <v>70</v>
+      </c>
+      <c r="B53" t="s">
+        <v>182</v>
+      </c>
+      <c r="C53" t="s">
+        <v>182</v>
+      </c>
+      <c r="D53" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A54" t="s">
+        <v>70</v>
+      </c>
+      <c r="B54" t="s">
+        <v>183</v>
+      </c>
+      <c r="C54" t="s">
+        <v>183</v>
+      </c>
+      <c r="D54" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A55" t="s">
+        <v>70</v>
+      </c>
+      <c r="B55" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" t="s">
+        <v>75</v>
+      </c>
+      <c r="D55" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A56" t="s">
+        <v>70</v>
+      </c>
+      <c r="B56" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56" t="s">
+        <v>76</v>
+      </c>
+      <c r="D56" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" t="s">
+        <v>77</v>
+      </c>
+      <c r="C57" t="s">
+        <v>77</v>
+      </c>
+      <c r="D57" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" t="s">
+        <v>70</v>
+      </c>
+      <c r="B58" t="s">
+        <v>81</v>
+      </c>
+      <c r="C58" t="s">
+        <v>81</v>
+      </c>
+      <c r="D58" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B45">
-    <sortCondition ref="B14:B45"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:B49">
+    <sortCondition ref="B14:B49"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2806,10 +3202,10 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="1" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B2" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C2">
         <v>20210625</v>

</xml_diff>